<commit_message>
se conecta con firebase
</commit_message>
<xml_diff>
--- a/backend/data/Consolidacion_KPI.xlsx
+++ b/backend/data/Consolidacion_KPI.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Documentos\Programacion\KPIAtsa\backend\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEA15250-C045-43DD-8474-37559B17C921}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF984457-4B47-4C8F-9A9F-0E384B32D7EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -431,7 +431,7 @@
   <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="B11" sqref="B2:D11"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -616,7 +616,7 @@
   <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:D11"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -759,10 +759,10 @@
         <v>5000</v>
       </c>
       <c r="C10" s="1">
-        <v>2790</v>
+        <v>3800</v>
       </c>
       <c r="D10" s="1">
-        <v>2210</v>
+        <v>1200</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">

</xml_diff>